<commit_message>
completed test 9 with live chat date, added all tests to excel report
</commit_message>
<xml_diff>
--- a/Test_suits.xlsx
+++ b/Test_suits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artium\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artium\eclipse-workspace\nextG-proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F6FB14-4FE2-4944-BD8D-F3ED244CA25B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CC5EA8-9485-41B5-B748-8D7DA20A1C64}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4238711C-3D58-4773-AB03-42F154A83EC0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4238711C-3D58-4773-AB03-42F154A83EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="test-suite-1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="120">
   <si>
     <t>Step</t>
   </si>
@@ -77,18 +77,6 @@
     <t>expectedWordInResultSunglasses: "Sunglasses";</t>
   </si>
   <si>
-    <t>"com.next.proj.nextG_proj.tests.DataProviderSearchingTest".</t>
-  </si>
-  <si>
-    <t>"com.next.proj.nextG_proj.tests.SearchProductTest".</t>
-  </si>
-  <si>
-    <t>"com.next.proj.nextG_proj.tests.SearchProductNegativeTest".</t>
-  </si>
-  <si>
-    <t>"com.next.proj.nextG_proj.tests.AddItemToBagTest".</t>
-  </si>
-  <si>
     <t>test-suite-2 (Next Product Test)</t>
   </si>
   <si>
@@ -98,9 +86,6 @@
     <t>Add item to bag with licking on "Add To Bag" button.</t>
   </si>
   <si>
-    <t>"com.next.proj.nextG_proj.tests.CheckFavoritesCounterTest".</t>
-  </si>
-  <si>
     <t>Check counter, before adding favorite items.</t>
   </si>
   <si>
@@ -131,21 +116,12 @@
     <t>test-suite-3 (Next Account Tests)</t>
   </si>
   <si>
-    <t xml:space="preserve">"com.next.proj.nextG_proj.tests.LoginTest".  </t>
-  </si>
-  <si>
-    <t>"com.next.proj.nextG_proj.tests.ChangeAccountDetailsTest".</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Assert that the old address and the new address are not equal.</t>
   </si>
   <si>
     <t>Click to State Or Province field, select Province with random and click on "Update" button.</t>
   </si>
   <si>
-    <t>"com.next.proj.nextG_proj.tests.ChangePasswordTest" .</t>
-  </si>
-  <si>
     <t>Enter new password and click "UPDATE" button.</t>
   </si>
   <si>
@@ -158,12 +134,6 @@
     <t>Check "Password validation message" and confirm the correct message .</t>
   </si>
   <si>
-    <t>Reenter new password and click on "UPDATE" button.</t>
-  </si>
-  <si>
-    <t>Get Result Title By Id.</t>
-  </si>
-  <si>
     <t>Confirm with message, that the request is match the search result.</t>
   </si>
   <si>
@@ -543,9 +513,6 @@
     </r>
   </si>
   <si>
-    <t>"com.next.proj.nextG_proj.tests.CheckFavoritesIconTest".</t>
-  </si>
-  <si>
     <t>"Favourite Icon" counter data saved .</t>
   </si>
   <si>
@@ -1463,6 +1430,335 @@
   </si>
   <si>
     <t>The expected message ("Sorry, we were unable to log in".) Must match the actual message.</t>
+  </si>
+  <si>
+    <t>Reenter new password and click on "Sign In Now " button</t>
+  </si>
+  <si>
+    <t>Get Result Title By Id and assert that the results title matches the search item string</t>
+  </si>
+  <si>
+    <t>Get Result Title Assert that the results title matches the search item string</t>
+  </si>
+  <si>
+    <t>_002_searchProductNegativeTest</t>
+  </si>
+  <si>
+    <t>_001_searchProductsTest</t>
+  </si>
+  <si>
+    <t>_004_addItemsToBagTest</t>
+  </si>
+  <si>
+    <t>_005_CheckFavoritesCounterTest</t>
+  </si>
+  <si>
+    <t>_006_CheckFavoritesIconTest</t>
+  </si>
+  <si>
+    <t>_007_LoginTest</t>
+  </si>
+  <si>
+    <t>_008_ChangeAccountDetailsTest</t>
+  </si>
+  <si>
+    <t>_010_ChangePasswordTest</t>
+  </si>
+  <si>
+    <t>_009_dateLiveChatTest</t>
+  </si>
+  <si>
+    <t>_003_searchFromMainLandingPageTest</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on the help button, switch to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">customer services </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> window</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switched from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>landing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">customer services  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page window.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switched from the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">customer services </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>live chat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page window.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on the chat button, switch to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>live chat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> window.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Get date from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>live chat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> window, get current date, assert that chat date and current date are equal.</t>
+    </r>
+  </si>
+  <si>
+    <t>The expected result is a message confirming that the assertion was true and the chat date is equal to the current date.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Close </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">live chat </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">page window, close  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>customer services page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> window, switch to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>landing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">next.co.il </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>landing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page,loaded.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1500,7 +1796,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1521,12 +1817,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1927,14 +2217,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2297,8 +2587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B799318-9110-4ADF-89BB-456A6F9FCB9E}">
   <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,7 +2611,7 @@
     </row>
     <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
@@ -2348,10 +2638,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="7"/>
@@ -2361,10 +2651,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="8"/>
@@ -2377,7 +2667,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
@@ -2387,10 +2677,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>7</v>
@@ -2402,10 +2692,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="8"/>
@@ -2415,10 +2705,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>8</v>
@@ -2433,14 +2723,14 @@
         <v>5</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="49" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
@@ -2467,10 +2757,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="20"/>
@@ -2480,10 +2770,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="22"/>
@@ -2496,7 +2786,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="22"/>
@@ -2506,10 +2796,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>12</v>
@@ -2524,7 +2814,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>13</v>
@@ -2535,18 +2825,18 @@
       <c r="A18" s="3">
         <v>6</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="40" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="52" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="B19" s="53"/>
       <c r="C19" s="53"/>
@@ -2573,10 +2863,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="20"/>
@@ -2586,22 +2876,24 @@
         <v>2</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="22"/>
     </row>
-    <row r="23" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>3</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="40"/>
+      <c r="B23" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>101</v>
+      </c>
       <c r="D23" s="12"/>
       <c r="E23" s="22"/>
     </row>
@@ -2884,10 +3176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F93C1BC-A027-4C59-A555-154DF687E5EF}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2901,7 +3193,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="46" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
@@ -2910,7 +3202,7 @@
     </row>
     <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="52" t="s">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
@@ -2930,17 +3222,17 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="42"/>
+      <c r="E3" s="41"/>
     </row>
     <row r="4" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
@@ -2950,10 +3242,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="8"/>
@@ -2963,10 +3255,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="8"/>
@@ -2976,10 +3268,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="8"/>
@@ -2989,10 +3281,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="8"/>
@@ -3002,10 +3294,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="8"/>
@@ -3015,10 +3307,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="8"/>
@@ -3028,10 +3320,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="8"/>
@@ -3041,10 +3333,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="8"/>
@@ -3057,14 +3349,14 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="52" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="B14" s="53"/>
       <c r="C14" s="53"/>
@@ -3084,17 +3376,17 @@
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="42"/>
+      <c r="E15" s="41"/>
     </row>
     <row r="16" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>1</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
@@ -3104,10 +3396,10 @@
         <v>2</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
@@ -3117,10 +3409,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
@@ -3130,23 +3422,23 @@
         <v>4</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>5</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>22</v>
+      <c r="B20" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
@@ -3156,13 +3448,13 @@
         <v>6</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E21" s="7"/>
     </row>
@@ -3171,10 +3463,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C22" s="39" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
@@ -3184,10 +3476,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
@@ -3200,14 +3492,14 @@
         <v>11</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="52" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
@@ -3227,17 +3519,17 @@
       <c r="D26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="42"/>
+      <c r="E26" s="41"/>
     </row>
     <row r="27" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>1</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
@@ -3247,10 +3539,10 @@
         <v>2</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="7"/>
@@ -3260,10 +3552,10 @@
         <v>3</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
@@ -3273,10 +3565,10 @@
         <v>4</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
@@ -3286,13 +3578,13 @@
         <v>5</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E31" s="7"/>
     </row>
@@ -3301,10 +3593,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
@@ -3314,44 +3606,135 @@
         <v>7</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>8</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="7"/>
     </row>
+    <row r="35" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="54"/>
+    </row>
+    <row r="36" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="41"/>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>1</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>2</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>3</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>4</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="7"/>
+    </row>
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>5</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A35:E35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CADE14E-8759-4498-B983-534DEBD5CAC8}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3364,7 +3747,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -3373,7 +3756,7 @@
     </row>
     <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="52" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
@@ -3393,17 +3776,17 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="42"/>
+      <c r="E3" s="41"/>
     </row>
     <row r="4" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
@@ -3416,7 +3799,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
@@ -3426,10 +3809,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
@@ -3439,10 +3822,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
@@ -3455,14 +3838,14 @@
         <v>11</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="52" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="B9" s="53"/>
       <c r="C9" s="53"/>
@@ -3482,17 +3865,17 @@
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="42"/>
+      <c r="E10" s="41"/>
     </row>
     <row r="11" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
@@ -3502,10 +3885,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
@@ -3515,10 +3898,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
@@ -3528,10 +3911,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
@@ -3541,10 +3924,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
@@ -3554,10 +3937,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
@@ -3567,15 +3950,15 @@
         <v>7</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>8</v>
       </c>
@@ -3583,168 +3966,175 @@
         <v>11</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
-    </row>
-    <row r="20" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="19" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="54"/>
+    </row>
+    <row r="27" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="42"/>
-    </row>
-    <row r="21" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="E27" s="41"/>
+    </row>
+    <row r="28" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>1</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>2</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>3</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>4</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>5</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>6</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>7</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>8</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="39" t="s">
-        <v>109</v>
+      <c r="B28" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>54</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>9</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>81</v>
+        <v>2</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
     </row>
+    <row r="31" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>4</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>5</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>6</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>7</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>8</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>9</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>10</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A26:E26"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A9:E9"/>

</xml_diff>

<commit_message>
added report to excel
</commit_message>
<xml_diff>
--- a/Test_suits.xlsx
+++ b/Test_suits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artium\eclipse-workspace\nextG-proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3181DA-3057-4FB3-BEFD-F13585481985}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD335D5F-6FEC-4FC8-A12D-1B214FEDB3B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{4238711C-3D58-4773-AB03-42F154A83EC0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4238711C-3D58-4773-AB03-42F154A83EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Report_sheet" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="138">
   <si>
     <t>Step</t>
   </si>
@@ -1751,13 +1751,70 @@
   </si>
   <si>
     <t>Click on "My Account link active" button, then click on "My Account SignOut" button.</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Galina Khononov</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>John Bryce Automation course</t>
+  </si>
+  <si>
+    <t>galinaltman@gmail.com</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>www.next.co.il/en</t>
+  </si>
+  <si>
+    <t>Website for the project</t>
+  </si>
+  <si>
+    <t>Project name</t>
+  </si>
+  <si>
+    <t>nextG-proj</t>
+  </si>
+  <si>
+    <t>A screenshot is taken after every test but the function is described only in one test in the report, where it is an actual part of the test.</t>
+  </si>
+  <si>
+    <t>There is a change password test that updates the password. There is no need to manually update the password in the configuration file, it is updated automatically in the code.</t>
+  </si>
+  <si>
+    <t>There are 3 test suites in the project.</t>
+  </si>
+  <si>
+    <t>The test suites can be run in any order.</t>
+  </si>
+  <si>
+    <t>Project github link</t>
+  </si>
+  <si>
+    <t>https://github.com/Galia99/next-proj.git</t>
+  </si>
+  <si>
+    <t>Username and password can be seen in the difido report.</t>
+  </si>
+  <si>
+    <t>To run the test suites, TestNG needs to be installed in the development environment (eclipse or IntelliJ).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1783,6 +1840,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2183,14 +2254,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2204,51 +2273,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2355,8 +2379,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2669,305 +2749,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B799318-9110-4ADF-89BB-456A6F9FCB9E}">
-  <dimension ref="A4:E114"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="62.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="64" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="63" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="66"/>
+      <c r="B8" s="62" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="66"/>
+      <c r="B9" s="65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="66"/>
+      <c r="B10" s="65" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="66"/>
+      <c r="B11" s="65" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="66"/>
+      <c r="B12" s="65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="62.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="61.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="4"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="3"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="4"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="3"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="2"/>
+    <row r="50" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="61.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
       <c r="D84" s="2"/>
-      <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="4"/>
-      <c r="C85" s="2"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
       <c r="D85" s="2"/>
-      <c r="E85" s="3"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="2"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
       <c r="D86" s="2"/>
-      <c r="E86" s="3"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="2"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
       <c r="D87" s="2"/>
-      <c r="E87" s="3"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="2"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
       <c r="D88" s="2"/>
-      <c r="E88" s="3"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="2"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="3"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="2"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
       <c r="D90" s="2"/>
-      <c r="E90" s="3"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="2"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
       <c r="D91" s="2"/>
-      <c r="E91" s="3"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="2"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
       <c r="D92" s="2"/>
-      <c r="E92" s="3"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="4"/>
-      <c r="C93" s="2"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
       <c r="D93" s="2"/>
-      <c r="E93" s="3"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="2"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
       <c r="D94" s="2"/>
-      <c r="E94" s="3"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-      <c r="B95" s="4"/>
-      <c r="C95" s="2"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="3"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="B96" s="4"/>
-      <c r="C96" s="2"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="3"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="2"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="3"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="2"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
       <c r="D98" s="2"/>
-      <c r="E98" s="3"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="2"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
       <c r="D99" s="2"/>
-      <c r="E99" s="3"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="4"/>
-      <c r="C100" s="2"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
       <c r="D100" s="2"/>
-      <c r="E100" s="3"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="4"/>
-      <c r="C101" s="2"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
       <c r="D101" s="2"/>
-      <c r="E101" s="3"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="4"/>
-      <c r="C102" s="2"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
       <c r="D102" s="2"/>
-      <c r="E102" s="3"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="2"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
       <c r="D103" s="2"/>
-      <c r="E103" s="3"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="4"/>
-      <c r="C104" s="2"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
       <c r="D104" s="2"/>
-      <c r="E104" s="3"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="4"/>
-      <c r="C105" s="2"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
       <c r="D105" s="2"/>
-      <c r="E105" s="3"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="4"/>
-      <c r="C106" s="2"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
       <c r="D106" s="2"/>
-      <c r="E106" s="3"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="2"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="3"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
       <c r="D107" s="2"/>
-      <c r="E107" s="3"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="4"/>
-      <c r="C108" s="2"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="3"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
       <c r="D108" s="2"/>
-      <c r="E108" s="3"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="2"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="3"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
       <c r="D109" s="2"/>
-      <c r="E109" s="3"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="2"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="3"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
       <c r="D110" s="2"/>
-      <c r="E110" s="3"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="4"/>
-      <c r="C111" s="2"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="3"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
       <c r="D111" s="2"/>
-      <c r="E111" s="3"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="2"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="3"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
       <c r="D112" s="2"/>
-      <c r="E112" s="3"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="2"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="3"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
       <c r="D113" s="2"/>
-      <c r="E113" s="3"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="2"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="3"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
       <c r="D114" s="2"/>
-      <c r="E114" s="3"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="3"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="2"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="3"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:A12"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{62C5C509-5641-4D70-8B8E-EBC353E6783E}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{0246E67D-505C-4E61-BB66-5005D277FD74}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{61C78107-8E93-4A41-8960-5F969DEEA61D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -2977,8 +3110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F93C1BC-A027-4C59-A555-154DF687E5EF}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2990,278 +3123,278 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+      <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="53"/>
+      <c r="D4" s="37"/>
     </row>
     <row r="5" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="A5" s="12">
         <v>2</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="38"/>
     </row>
     <row r="6" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28">
+      <c r="A6" s="12">
         <v>3</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="54"/>
+      <c r="D6" s="38"/>
     </row>
     <row r="7" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="A7" s="12">
         <v>4</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="45" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28">
+      <c r="A8" s="12">
         <v>5</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="54"/>
+      <c r="D8" s="38"/>
     </row>
     <row r="9" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9" s="12">
         <v>6</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="39" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="33">
+      <c r="A10" s="17">
         <v>7</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="56"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="54"/>
     </row>
     <row r="12" spans="1:4" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+      <c r="A13" s="12">
         <v>1</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="53"/>
+      <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="37">
+      <c r="A14" s="21">
         <v>2</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="54"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37">
+      <c r="A15" s="21">
         <v>3</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="54"/>
+      <c r="D15" s="38"/>
     </row>
     <row r="16" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37">
+      <c r="A16" s="21">
         <v>4</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D16" s="38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37">
+      <c r="A17" s="21">
         <v>5</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="39" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="11">
         <v>6</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="56"/>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" spans="1:4" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
+      <c r="A21" s="12">
         <v>1</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="53"/>
+      <c r="D21" s="37"/>
     </row>
     <row r="22" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37">
+      <c r="A22" s="21">
         <v>2</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="54"/>
+      <c r="D22" s="38"/>
     </row>
     <row r="23" spans="1:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="57">
+      <c r="A23" s="41">
         <v>3</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="59" t="s">
+      <c r="C23" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="60"/>
+      <c r="D23" s="44"/>
     </row>
     <row r="24" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3301,488 +3434,488 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+      <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37">
+      <c r="A5" s="21">
         <v>2</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37">
+      <c r="A6" s="21">
         <v>3</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37">
+      <c r="A7" s="21">
         <v>4</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
+      <c r="A8" s="21">
         <v>5</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="30"/>
+      <c r="D8" s="14"/>
     </row>
     <row r="9" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37">
+      <c r="A9" s="21">
         <v>6</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37">
+      <c r="A10" s="21">
         <v>7</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="30"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37">
+      <c r="A11" s="21">
         <v>8</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37">
+      <c r="A12" s="21">
         <v>9</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27">
+      <c r="A13" s="11">
         <v>10</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="35"/>
+      <c r="D13" s="19"/>
     </row>
     <row r="14" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
     </row>
     <row r="15" spans="1:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28">
+      <c r="A16" s="12">
         <v>1</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="12">
         <v>2</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="29"/>
+      <c r="D17" s="13"/>
     </row>
     <row r="18" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28">
+      <c r="A18" s="12">
         <v>3</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="29"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28">
+      <c r="A19" s="12">
         <v>4</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="29"/>
+      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28">
+      <c r="A20" s="12">
         <v>5</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="29"/>
+      <c r="D20" s="13"/>
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
+      <c r="A21" s="12">
         <v>6</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28">
+      <c r="A22" s="12">
         <v>7</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D22" s="29"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28">
+      <c r="A23" s="12">
         <v>8</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C23" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="29"/>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28">
+      <c r="A24" s="12">
         <v>9</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="29"/>
+      <c r="D24" s="13"/>
     </row>
     <row r="25" spans="1:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="28">
+      <c r="A27" s="12">
         <v>1</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="13"/>
     </row>
     <row r="28" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="28">
+      <c r="A28" s="12">
         <v>2</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="29"/>
+      <c r="D28" s="13"/>
     </row>
     <row r="29" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28">
+      <c r="A29" s="12">
         <v>3</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="28">
+      <c r="A30" s="12">
         <v>4</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="29"/>
+      <c r="D30" s="13"/>
     </row>
     <row r="31" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="28">
+      <c r="A31" s="12">
         <v>5</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="53" t="s">
+      <c r="D31" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28">
+      <c r="A32" s="12">
         <v>6</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="48" t="s">
+      <c r="C32" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="29"/>
+      <c r="D32" s="13"/>
     </row>
     <row r="33" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28">
+      <c r="A33" s="12">
         <v>7</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="48" t="s">
+      <c r="C33" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="29"/>
+      <c r="D33" s="13"/>
     </row>
     <row r="34" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="28">
+      <c r="A34" s="12">
         <v>8</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="50" t="s">
+      <c r="C34" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="29"/>
+      <c r="D34" s="13"/>
     </row>
     <row r="35" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="57"/>
     </row>
     <row r="36" spans="1:4" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28">
+      <c r="A37" s="12">
         <v>1</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="29"/>
+      <c r="D37" s="13"/>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="28">
+      <c r="A38" s="12">
         <v>2</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="29"/>
+      <c r="D38" s="13"/>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="28">
+      <c r="A39" s="12">
         <v>3</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="50" t="s">
+      <c r="C39" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="29"/>
+      <c r="D39" s="13"/>
     </row>
     <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="28">
+      <c r="A40" s="12">
         <v>4</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B40" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="50" t="s">
+      <c r="C40" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="29"/>
+      <c r="D40" s="13"/>
     </row>
     <row r="41" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="5">
+      <c r="A41" s="4">
         <v>5</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="8"/>
+      <c r="D41" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3800,8 +3933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB13AF73-D8A3-44BF-92EE-CFC1B0137ABD}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3812,354 +3945,354 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+      <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="A5" s="12">
         <v>2</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28">
+      <c r="A6" s="12">
         <v>3</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="29"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="A7" s="12">
         <v>4</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33">
+      <c r="A8" s="17">
         <v>5</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="41"/>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="57"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
+      <c r="A11" s="12">
         <v>1</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="29"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28">
+      <c r="A12" s="12">
         <v>2</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="29"/>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+      <c r="A13" s="12">
         <v>3</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="29"/>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:4" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28">
+      <c r="A14" s="12">
         <v>4</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="29"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
+      <c r="A15" s="12">
         <v>5</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="29"/>
+      <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28">
+      <c r="A16" s="12">
         <v>6</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="12">
         <v>7</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="29"/>
+      <c r="D17" s="13"/>
     </row>
     <row r="18" spans="1:4" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>8</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
+      <c r="A21" s="12">
         <v>1</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="29"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="28">
+      <c r="A22" s="12">
         <v>2</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="29"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="28">
+      <c r="A23" s="12">
         <v>3</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C23" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="29"/>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="28">
+      <c r="A24" s="12">
         <v>4</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="29"/>
+      <c r="D24" s="13"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="28">
+      <c r="A25" s="12">
         <v>5</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="50" t="s">
+      <c r="C25" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="29"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="28">
+      <c r="A26" s="12">
         <v>6</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="29"/>
+      <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="28">
+      <c r="A27" s="12">
         <v>7</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="50" t="s">
+      <c r="C27" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="13"/>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="28">
+      <c r="A28" s="12">
         <v>8</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="50" t="s">
+      <c r="C28" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="29"/>
+      <c r="D28" s="13"/>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="28">
+      <c r="A29" s="12">
         <v>9</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="50" t="s">
+      <c r="C29" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>10</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="52" t="s">
+      <c r="C30" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="8"/>
+      <c r="D30" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>